<commit_message>
Finalizando Grafico de Pizza
</commit_message>
<xml_diff>
--- a/src/main/resources/gastos.xlsx
+++ b/src/main/resources/gastos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Janeiro</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>Alimentação</t>
-  </si>
-  <si>
-    <t>Viagens</t>
-  </si>
-  <si>
-    <t>Saúde</t>
   </si>
 </sst>
 </file>
@@ -55,7 +49,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +66,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -127,7 +129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -135,6 +137,7 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,51 +479,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5">
-        <v>480</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1250</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>240</v>
-      </c>
-      <c r="F3" s="5">
-        <v>850</v>
-      </c>
-      <c r="G3" s="5">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="5">
-        <v>290</v>
-      </c>
-      <c r="C4" s="5">
-        <v>290</v>
-      </c>
-      <c r="D4" s="5">
-        <v>410</v>
-      </c>
-      <c r="E4" s="5">
-        <v>150</v>
-      </c>
-      <c r="F4" s="5">
-        <v>315</v>
-      </c>
-      <c r="G4" s="5">
-        <v>632</v>
-      </c>
+    <row r="11" spans="1:7" ht="16.2" x14ac:dyDescent="0.45">
+      <c r="F11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>